<commit_message>
Merge error cronogramas e proto at-oa/at-oa.bmpr
</commit_message>
<xml_diff>
--- a/Cronogramas.xlsx
+++ b/Cronogramas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma Telas" sheetId="1" r:id="rId1"/>
@@ -537,7 +537,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -547,7 +547,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
@@ -976,8 +976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -987,7 +987,7 @@
     <col min="3" max="3" width="25.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>